<commit_message>
Activity 6 first draft
</commit_message>
<xml_diff>
--- a/data/CrimeTotals.xlsx
+++ b/data/CrimeTotals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="460" windowWidth="23980" windowHeight="12500" tabRatio="500"/>
+    <workbookView xWindow="2140" yWindow="660" windowWidth="23980" windowHeight="12500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,6 +597,12 @@
       <c r="G4">
         <v>87</v>
       </c>
+      <c r="H4">
+        <v>89</v>
+      </c>
+      <c r="I4">
+        <v>90</v>
+      </c>
       <c r="J4" s="1">
         <v>10.7</v>
       </c>

</xml_diff>